<commit_message>
Review 10 Problems 1/27/2026
</commit_message>
<xml_diff>
--- a/Code & Notes/Functions & Notes.xlsx
+++ b/Code & Notes/Functions & Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Tracks &amp; Courses\Web Development\Problem Solving\Code &amp; Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\Code &amp; Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62350279-205A-4D43-B672-2FEEC08FE251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91DA777-0C1A-4DC7-AE3D-C088F09C8C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript" sheetId="1" r:id="rId1"/>
@@ -794,15 +794,51 @@
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -811,42 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,17 +1136,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="91" customWidth="1"/>
     <col min="2" max="2" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>92</v>
       </c>
@@ -1154,13 +1154,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="47"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="41"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1176,13 +1176,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="51"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="46"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>131</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>133</v>
       </c>
@@ -1230,13 +1230,13 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="52"/>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1244,13 +1244,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="53"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="48"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>23</v>
       </c>
@@ -1266,13 +1266,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="48"/>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>64</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>16</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>48</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>10</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>104</v>
       </c>
@@ -1320,13 +1320,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="54" t="s">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="54"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="49"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
         <v>25</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>65</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>66</v>
       </c>
@@ -1358,13 +1358,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="55" t="s">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="55"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>17</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>68</v>
       </c>
@@ -1380,13 +1380,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="56"/>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="51"/>
+    </row>
+    <row r="33" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>72</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>73</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="19" t="s">
         <v>57</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="19" t="s">
         <v>49</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
         <v>117</v>
       </c>
@@ -1426,13 +1426,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="57"/>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="52"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>33</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="26" t="s">
         <v>35</v>
       </c>
@@ -1448,13 +1448,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="58" t="s">
+    <row r="41" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="58"/>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="53"/>
+    </row>
+    <row r="42" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="29" t="s">
         <v>29</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="30" t="s">
         <v>122</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="31" t="s">
         <v>27</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
         <v>31</v>
       </c>
@@ -1486,19 +1486,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="43"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="44"/>
+      <c r="B47" s="45"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="31" t="s">
         <v>46</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="31" t="s">
         <v>124</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="31" t="s">
         <v>111</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="29" t="s">
         <v>41</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="29" t="s">
         <v>75</v>
       </c>
@@ -1538,27 +1538,27 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="45" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
-      <c r="B54" s="43"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="43"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="55"/>
+      <c r="B54" s="45"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="55"/>
+      <c r="B55" s="45"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="55"/>
+      <c r="B56" s="45"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="31" t="s">
         <v>96</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="31" t="s">
         <v>98</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="31" t="s">
         <v>112</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="31" t="s">
         <v>137</v>
       </c>
@@ -1590,13 +1590,13 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="44" t="s">
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="44"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="56"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="32" t="s">
         <v>61</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="34" t="s">
         <v>59</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="32" t="s">
         <v>83</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="36" t="s">
         <v>103</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="36" t="s">
         <v>121</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="36" t="s">
         <v>109</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="36" t="s">
         <v>139</v>
       </c>
@@ -1652,13 +1652,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="46" t="s">
+    <row r="69" spans="1:2" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B69" s="46"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="58"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="21" t="s">
         <v>75</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="23" t="s">
         <v>45</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="21" t="s">
         <v>53</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="21" t="s">
         <v>77</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="23" t="s">
         <v>70</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="23" t="s">
         <v>51</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="23" t="s">
         <v>100</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="23" t="s">
         <v>106</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="38" t="s">
         <v>118</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="23" t="s">
         <v>125</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="23" t="s">
         <v>135</v>
       </c>
@@ -1746,13 +1746,13 @@
         <v>136</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="45" t="s">
+    <row r="81" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A81" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="B81" s="45"/>
-    </row>
-    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="57"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="39" t="s">
         <v>129</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="39" t="s">
         <v>129</v>
       </c>
@@ -1770,6 +1770,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A46:A47"/>
@@ -1782,11 +1787,6 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A69:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>